<commit_message>
Add simple GUI, warning message, show data , clear data
</commit_message>
<xml_diff>
--- a/Database.xlsx
+++ b/Database.xlsx
@@ -3,12 +3,18 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="1440" yWindow="-14760" windowWidth="21600" windowHeight="11325" tabRatio="600" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="600" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="Peerapat" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="Chanakarn" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Teerapat" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="Teerapat1" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="Teerapat2" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="Jarukit" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="Suthichai" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="Wiwat" sheetId="9" state="visible" r:id="rId9"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -437,10 +443,139 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="A3:E11"/>
+      <selection activeCell="A3" sqref="A3:XFD6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
+  <cols>
+    <col width="18.109375" bestFit="1" customWidth="1" min="1" max="1"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Peerapat</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Time</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Weight</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Height</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>BMI</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="2" t="n">
+        <v>44471.97650728009</v>
+      </c>
+      <c r="B3" t="n">
+        <v>66</v>
+      </c>
+      <c r="C3" t="n">
+        <v>170</v>
+      </c>
+      <c r="D3" t="n">
+        <v>22.84</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>03/10/2021 01:23</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>57</v>
+      </c>
+      <c r="C4" t="n">
+        <v>155</v>
+      </c>
+      <c r="D4" t="n">
+        <v>23.73</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>03/10/2021 01:23</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>67</v>
+      </c>
+      <c r="C5" t="n">
+        <v>178</v>
+      </c>
+      <c r="D5" t="n">
+        <v>21.15</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>03/10/2021 01:23</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>46</v>
+      </c>
+      <c r="C6" t="n">
+        <v>167</v>
+      </c>
+      <c r="D6" t="n">
+        <v>16.49</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>03/10/2021 01:49</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>66</v>
+      </c>
+      <c r="C7" t="n">
+        <v>180</v>
+      </c>
+      <c r="D7" t="n">
+        <v>20.37</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.4"/>
@@ -448,7 +583,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>Peerapat</t>
+          <t>Chanakarn</t>
         </is>
       </c>
     </row>
@@ -475,51 +610,31 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="1" t="n"/>
-    </row>
-    <row r="7">
-      <c r="A7" s="1" t="n"/>
-    </row>
-    <row r="8">
-      <c r="A8" s="2" t="n">
-        <v>44471.03258289352</v>
-      </c>
-      <c r="B8" t="n">
-        <v>60</v>
-      </c>
-      <c r="C8" t="n">
-        <v>170</v>
-      </c>
-      <c r="D8" t="n">
-        <v>20.76124567474049</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" s="2" t="n">
-        <v>44471.03282131944</v>
-      </c>
-      <c r="B9" t="n">
-        <v>55</v>
-      </c>
-      <c r="C9" t="n">
-        <v>170</v>
-      </c>
-      <c r="D9" t="n">
-        <v>19.03114186851211</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="2" t="n">
-        <v>44471.03304798611</v>
-      </c>
-      <c r="B10" t="n">
-        <v>63</v>
-      </c>
-      <c r="C10" t="n">
-        <v>170</v>
-      </c>
-      <c r="D10" t="n">
-        <v>21.79930795847751</v>
+      <c r="A3" s="1" t="n">
+        <v>44471.03380539352</v>
+      </c>
+      <c r="B3" t="n">
+        <v>40</v>
+      </c>
+      <c r="C3" t="n">
+        <v>155</v>
+      </c>
+      <c r="D3" t="n">
+        <v>16.64932362122789</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="n">
+        <v>44471.03458726852</v>
+      </c>
+      <c r="B4" t="n">
+        <v>39</v>
+      </c>
+      <c r="C4" t="n">
+        <v>155</v>
+      </c>
+      <c r="D4" t="n">
+        <v>16.23309053069719</v>
       </c>
     </row>
   </sheetData>
@@ -527,7 +642,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -544,7 +659,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>Chanakarn</t>
+          <t>Teerapat</t>
         </is>
       </c>
     </row>
@@ -572,30 +687,312 @@
     </row>
     <row r="3">
       <c r="A3" s="2" t="n">
-        <v>44471.03380539352</v>
+        <v>44471.98242291667</v>
       </c>
       <c r="B3" t="n">
-        <v>40</v>
+        <v>60</v>
       </c>
       <c r="C3" t="n">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="D3" t="n">
-        <v>16.64932362122789</v>
+        <v>26.67</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="n">
-        <v>44471.03458727109</v>
+        <v>44471.98256384259</v>
       </c>
       <c r="B4" t="n">
-        <v>39</v>
+        <v>56</v>
       </c>
       <c r="C4" t="n">
-        <v>155</v>
+        <v>179</v>
       </c>
       <c r="D4" t="n">
-        <v>16.23309053069719</v>
+        <v>17.48</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Teerapat</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Time</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Weight</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Height</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>BMI</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="2" t="n">
+        <v>44471.98162346065</v>
+      </c>
+      <c r="B3" t="n">
+        <v>60</v>
+      </c>
+      <c r="C3" t="n">
+        <v>160</v>
+      </c>
+      <c r="D3" t="n">
+        <v>23.44</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Teerapat</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Time</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Weight</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Height</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>BMI</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="2" t="n">
+        <v>44471.98167570602</v>
+      </c>
+      <c r="B3" t="n">
+        <v>60</v>
+      </c>
+      <c r="C3" t="n">
+        <v>160</v>
+      </c>
+      <c r="D3" t="n">
+        <v>23.44</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Jarukit</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Time</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Weight</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Height</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>BMI</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Suthichai</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Time</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Weight</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Height</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>BMI</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="2" t="n">
+        <v>44472.02924034722</v>
+      </c>
+      <c r="B3" t="n">
+        <v>60</v>
+      </c>
+      <c r="C3" t="n">
+        <v>170</v>
+      </c>
+      <c r="D3" t="n">
+        <v>20.76</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Wiwat</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Time</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Weight</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Height</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>BMI</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>